<commit_message>
Restructured CurateDataDS, Bugfixing, worked on AugmentDataDS, Ver 0.1.12
</commit_message>
<xml_diff>
--- a/Development/ToDo.xlsx
+++ b/Development/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2E6F5D-90DD-4B2F-A3FB-E8E141C2F3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F2CA25-7AC6-49CE-BF22-8F6DDF639469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,10 +45,10 @@
     <t>GetValidationReportDS</t>
   </si>
   <si>
-    <t>In allen Tabellen Zeilen rausschmeißen, zu denen es keine passende Diagnosis- und Patient-Data gibtr</t>
+    <t>in Events: Daten für initiale Diagnose und LastVitalStatus ggf. anpassen, falls nicht konsistent mit anderen verfügbaren Daten</t>
   </si>
   <si>
-    <t>Duplikate in allen Tabellen</t>
+    <t>Bei InitialDiagnosis: Diagnose-Details zu nestes Details</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -414,12 +414,12 @@
     </row>
     <row r="5" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reimplementation of transformation tracking
</commit_message>
<xml_diff>
--- a/Development/ToDo.xlsx
+++ b/Development/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840F8A1E-61A5-4558-A1EE-88025841496E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759E57CD-1095-4516-BCD8-11DB3A479248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Task</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>renv implementieren</t>
-  </si>
-  <si>
-    <t>Monitor data frames: Add column with transformed value (Zuordnung ursprüngliches zu transformiertem Wert ermöglichen)</t>
   </si>
   <si>
     <t>Validierungs-Funktionen direkt an ds.CurateData und ds.AugmentData anhängen</t>
@@ -415,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -479,19 +476,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="20" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on session object meta data akquisition
</commit_message>
<xml_diff>
--- a/Development/ToDo.xlsx
+++ b/Development/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759E57CD-1095-4516-BCD8-11DB3A479248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21F380F-9F3F-4A17-BA52-F1A645534B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Task</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>GetValidationReportDS</t>
-  </si>
-  <si>
-    <t>in Events: Daten für initiale Diagnose und LastVitalStatus ggf. anpassen, falls nicht konsistent mit anderen verfügbaren Daten</t>
-  </si>
-  <si>
-    <t>Bei InitialDiagnosis: Diagnose-Details zu nested Details</t>
   </si>
   <si>
     <t>Checken Selektion in CCP-Explorer: Werden bei multiplen Malignomen alle Fälle von Patienten mitselektiert?</t>
@@ -412,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -438,52 +432,42 @@
     </row>
     <row r="4" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ver 0.1.40: Major changes in data model
</commit_message>
<xml_diff>
--- a/Development/ToDo.xlsx
+++ b/Development/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21F380F-9F3F-4A17-BA52-F1A645534B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07389CE-765B-4F60-8667-48AFADC3DF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Task</t>
-  </si>
-  <si>
-    <t>Check function: feature names in RDS correct? All tables and features available?</t>
-  </si>
-  <si>
-    <t>GetValidationReportDS</t>
   </si>
   <si>
     <t>Checken Selektion in CCP-Explorer: Werden bei multiplen Malignomen alle Fälle von Patienten mitselektiert?</t>
@@ -404,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C22"/>
+  <dimension ref="B2:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -417,57 +411,49 @@
     <col min="3" max="16384" width="17.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="14" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+    <row r="16" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>